<commit_message>
add prime number checking
</commit_message>
<xml_diff>
--- a/full-stack-challenge.xlsx
+++ b/full-stack-challenge.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448"/>
   </bookViews>
   <sheets>
     <sheet name="Foundations of JavaScript" sheetId="1" r:id="rId1"/>
@@ -2438,7 +2438,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2454,6 +2454,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2522,7 +2528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2575,6 +2581,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3161,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3263,10 +3275,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="13" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21" t="s">
         <v>408</v>
       </c>
     </row>
@@ -3282,7 +3294,7 @@
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="13" t="s">
         <v>409</v>
       </c>
     </row>
@@ -4257,7 +4269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add logo to menu items
</commit_message>
<xml_diff>
--- a/full-stack-challenge.xlsx
+++ b/full-stack-challenge.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Full Stack Dev. Challenge\Full-Stack-Dev.-Challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Full-Stack-Dev.-Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foundations of JavaScript" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="536">
   <si>
     <t>Challenge Number</t>
   </si>
@@ -2384,12 +2384,214 @@
 Use the callback function to perform a specific operation on the two numbers, such as addition, subtraction, multiplication, or division.
 Test the higher-order function by passing different callback functions to perform various arithmetic operations.</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Event Listener Higher-Order Function
+Question: Implement a higher-order function in Kotlin that allows for easy handling of button click events across multiple views. The function should accept a lambda expression that defines what happens when a button is clicked. Demonstrate how this higher-order function simplifies adding click listeners to buttons in an Android application.</t>
+  </si>
+  <si>
+    <t>Set Operations with Higher-Order Functions
+Question: Define higher-order functions in Scheme that operate on sets represented as lists. Implement takewhile and dropwhile functions that manipulate lists based on a predicate. Provide examples demonstrating how these functions can be used to filter elements from a list according to a condition.</t>
+  </si>
+  <si>
+    <t>Ordered Lists and Comparison
+Question: Develop a higher-order function in Scheme called ordered-by, which takes a comparison function as input and returns a predicate function. This predicate checks whether a given list is totally ordered according to the comparison function. Include examples showing how ordered-by can be used with different comparison functions to validate the ordering of lists.</t>
+  </si>
+  <si>
+    <t>Utilizing Classic Higher-Order Functions
+Question: Without using recursion or case analysis in your definitions, create functions in Scheme that utilize map, curry, foldl, and foldr. These functions should operate on non-empty lists to find the maximum, sum, and product of integer elements within the list. Ensure your implementations correctly handle non-empty lists and produce scalar results.</t>
+  </si>
+  <si>
+    <t>Transforming Array Elements with .map()
+Objective: Understand and implement the .map() method to transform each element in an array.
+Details:
+Task Description: Write a JavaScript function that takes an array of numbers as input and returns a new array where each number has been multiplied by 2. Use the .map() method to achieve this transformation.
+Key Concepts: Focus on understanding how .map() works by applying a function to each element of an array and creating a new array with the results.
+Testing: After implementing the function, test it with an example array [1, 2, 3, 4] to ensure it correctly doubles each element.</t>
+  </si>
+  <si>
+    <t>Task 5: Custom Sorting with .sort()
+Objective: Explore the .sort() method for customizing the sorting order of an array.
+Details:
+Task Description: Given an array of objects representing people, write a function that sorts the array in ascending order based on the age property of each object. Use the .sort() method with a custom comparator function.
+Key Concepts: Understand how .sort() can be customized by passing a compare function to determine the sort order. Reflect on the importance of specifying a compare function for complex data structures.
+Testing: Test your function with an array of people objects to ensure they are sorted correctly by age.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 4: Iterating Over Array Elements with .forEach()
+Objective: Learn to use the .forEach() method for executing a function on each element of an array.
+Details:
+Task Description: Write a function that takes an array of strings and logs each string to the console. Use the .forEach() method to iterate over the array and perform the logging action.
+Key Concepts: Understand the purpose of .forEach() in executing a function for each element in an array without returning a new array. Consider the benefits of using .forEach() over traditional looping constructs.
+Testing: Test your function with an array ['Hello', 'World'] to see each string logged to the console.
+</t>
+  </si>
+  <si>
+    <t>Filtering Array Elements with .filter()
+Objective: Learn to use the .filter() method to select specific elements from an array.
+Details:
+Task Description: Write a function that takes an array of numbers and returns a new array containing only the even numbers from the original array. Use the .filter() method to identify and collect the even numbers.
+Key Concepts: Understand the role of .filter() in extracting elements based on a condition. Pay attention to how the callback function passed to .filter() determines which elements are included in the new array.
+Testing: Test your function with an array [1, 2, 3, 4, 5, 6] to verify that it correctly filters out the odd numbers.</t>
+  </si>
+  <si>
+    <t>Task 3: Accumulating Array Elements with .reduce()
+Objective: Practice using the .reduce() method to aggregate values from an array.
+Details:
+Task Description: Implement a function that calculates the sum of all numbers in an array. Use the .reduce() method to accumulate the sum as you iterate through the array.
+Key Concepts: Focus on how .reduce() works by applying a function to each element of an array and accumulating a result. Understand the initial value parameter and how it affects the calculation.
+Testing: Test your function with an array [1, 2, 3, 4, 5] to confirm it accurately sums up all the numbers.</t>
+  </si>
+  <si>
+    <t>Creating and Exporting Variables
+Objective: Learn how to create and export variables using ES6 module syntax.
+Details:
+Task Description: Write a JavaScript module that exports a constant array of numbers. Use the export keyword to make the array accessible to other modules.
+Key Concepts: Understand the use of export to expose variables, functions, or classes from a module. Pay attention to the difference between exporting individual members and exporting them all at once.
+Testing: After exporting the array, try importing it in another module to verify that it can be accessed and used.</t>
+  </si>
+  <si>
+    <t>Defining and Exporting a Function
+Objective: Practice defining and exporting a function using ES6 module syntax.
+Details:
+Task Description: Create a module that exports a function. This function should take a message as an argument and log it to the console. Use the export keyword to define the function's availability outside the module.
+Key Concepts: Focus on the syntax for exporting functions and the implications of making them part of the module's public interface.
+Testing: Import the function in another module and call it with a sample message to check its functionality.</t>
+  </si>
+  <si>
+    <t>Exporting a Class
+Objective: Learn how to define and export a class using ES6 module syntax.
+Details:
+Task Description: Write a module that exports a class. This class should have a constructor that initializes a greeting message. Use the export keyword to make the class available for instantiation in other modules.
+Key Concepts: Understand the process of exporting classes and the benefits of encapsulating functionality within classes.
+Testing: Import the class in another module, instantiate it, and call its methods to verify its functionality.</t>
+  </si>
+  <si>
+    <t>Importing Multiple Exports
+Objective: Learn how to import multiple exports from a module using ES6 import syntax.
+Details:
+Task Description: In a separate module, import both the array and the function exported from the previous tasks. Use the import statement to bring in the required exports.
+Key Concepts: Understand the syntax for importing multiple exports and the flexibility it offers in accessing different parts of a module.
+Testing: After importing, use the array and function in your module to demonstrate their functionality.</t>
+  </si>
+  <si>
+    <t>Default Export and Import
+Objective: Practice using default exports and imports in ES6 modules.
+Details:
+Task Description: Modify the module from Task 2 to use a default export instead of named exports. Then, adjust the import statement in Task 4 to import the default export.
+Key Concepts: Distinguish between default exports and named exports, and understand why and when to use each type.
+Testing: Verify that the default export behaves as expected when imported and used in another module.</t>
+  </si>
+  <si>
+    <t>Asynchronous File Reading with Callbacks:
+Write a program in Node.js that reads the content of a file asynchronously using the fs.readFile method. Use a callback function to handle the data once the file has been read. If the file read is successful, print the content to the console. If there is an error (e.g., the file does not exist), print an appropriate error message.
+Hint: Use fs.readFile('path/to/file', 'utf8', callback) from the fs module.</t>
+  </si>
+  <si>
+    <t>Event Handling in the Browser:
+Create an HTML page with a button. Write JavaScript code to handle the button click event using a callback function. When the button is clicked, display an alert with a custom message. Additionally, after the alert is dismissed, change the button text to "Clicked!".
+Hint: Use document.getElementById('button-id').addEventListener('click', callback)</t>
+  </si>
+  <si>
+    <t>Asynchronous API Call:
+Write a JavaScript function that makes an asynchronous HTTP GET request to a public API (e.g., JSONPlaceholder). Use the fetch API to get a list of posts. Pass a callback function to handle the response. The callback should parse the JSON data and log the titles of the posts to the console. If the request fails, log an error message.
+Hint: Use fetch('https://jsonplaceholder.typicode.com/posts').then(callback).catch(errorCallback).
+Custom Event Emitter</t>
+  </si>
+  <si>
+    <t>Custom Event Emitter:
+Implement a simple custom event emitter class in JavaScript. This class should have methods to register event listeners, emit events, and remove event listeners. Write a test case where you create an instance of this class, register a couple of callbacks for a custom event, emit the event, and ensure the callbacks are executed in order. Finally, demonstrate removing a listener and emitting the event again to show the listener is no longer called.
+Hint: Use an object to store events and their corresponding listeners.</t>
+  </si>
+  <si>
+    <t>Handling Multiple Asynchronous Operations:
+Write a JavaScript function that simulates fetching user data and their corresponding posts data asynchronously. Use callback functions to handle the data fetching. First, fetch the user data (e.g., from https://jsonplaceholder.typicode.com/users/1), then use the user's ID to fetch their posts (e.g., from https://jsonplaceholder.typicode.com/posts?userId=1). Print the user's name and the titles of their posts to the console. Handle any errors that occur during the fetch operations.
+Hint: Use nested fetch calls or the async/await syntax for a cleaner approach.</t>
+  </si>
+  <si>
+    <t>Dynamic List Item Handling:
+Create an HTML page with an unordered list (&lt;ul&gt;) and a button to add new list items (&lt;li&gt;). Use event delegation to handle click events on any list item. When a list item is clicked, display an alert with the text content of the clicked item. Ensure that newly added items are also handled by the same event listener.
+Hint: Attach a single click event listener to the parent &lt;ul&gt; element.</t>
+  </si>
+  <si>
+    <t>Form Input Validation:
+Implement a form with multiple input fields (e.g., text, email, number) and a submit button. Use event delegation to validate each input field when it loses focus (blur event). If the input is invalid, display an error message next to the field. Use a single event listener attached to the form element.
+Hint: Use the blur event and check the event target's validity using event.target.validity.</t>
+  </si>
+  <si>
+    <t>Menu Navigation:
+Create a navigation menu with nested submenus. Use event delegation to handle hover events to show or hide the submenus. When a submenu item is hovered over, display the corresponding submenu. Use a single event listener attached to the main menu.
+Hint: Use mouseover and mouseout events on the parent menu element to manage submenus.</t>
+  </si>
+  <si>
+    <t>Table Row Highlighting:
+Build a table with multiple rows. Use event delegation to highlight a table row when the mouse is over it and remove the highlight when the mouse leaves. Use a single event listener on the table element.
+Hint: Use the mouseover and mouseout events and check event.target to identify rows.</t>
+  </si>
+  <si>
+    <t>Delegated Event Removal:
+Create a to-do list where each item has a delete button. Use event delegation to handle the click event on the delete button to remove the corresponding list item. Ensure the event listener is attached to a parent element and dynamically handle items added after the initial page load.
+Hint: Attach the event listener to the parent &lt;ul&gt; element and use event.target to identify the delete button.</t>
+  </si>
+  <si>
+    <t>Pure Functions and Side Effects:
+Write a pure function increment that takes a number and returns the number incremented by 1 without modifying any external state. Contrast this with a function that increments a global variable. Explain the importance of pure functions and avoiding side effects in functional programming.
+Hint: Ensure increment has no side effects by not relying on or modifying external variables.</t>
+  </si>
+  <si>
+    <t>Map, Filter, and Reduce:
+Given an array of numbers, use the map, filter, and reduce functions to perform the following tasks:
+Double each number.
+Filter out numbers less than 10.
+Calculate the sum of the remaining numbers.
+Hint: Chain the map, filter, and reduce functions to achieve the result.</t>
+  </si>
+  <si>
+    <t>Immutability with Object.freeze:
+Create an object representing a user with properties like name and age. Use Object.freeze to make the object immutable. Attempt to change a property of the object and show that it remains unchanged. Explain why immutability is beneficial in functional programming.
+Hint: Use Object.freeze and try to mutate the object properties.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currying Example:
+Write a function add that can be used to add two numbers, but it should be curried. For example, add(2)(3) should return 5. Demonstrate the usage of this function by creating partially applied versions of the function to add specific numbers.
+Hint: Define a function that returns another function to achieve currying.
+</t>
+  </si>
+  <si>
+    <t>Function Composition:
+Implement two functions, double and square, that take a number and return its double and square, respectively. Create a function compose that takes two functions and returns their composition. Use compose to create a new function that first doubles a number and then squares it. Demonstrate this composed function with an example.
+Hint: The compose function should return a function that applies both functions in sequence.</t>
+  </si>
+  <si>
+    <t>Basic Try-Catch:
+Write a function that attempts to parse a JSON string. Use a try-catch block to handle any errors that occur during parsing. If an error occurs, return a default object with an error message. Demonstrate this function with valid and invalid JSON strings.
+Hint: Use JSON.parse inside the try block and return an error message in the catch block.</t>
+  </si>
+  <si>
+    <t>Custom Error Class:
+Create a custom error class ValidationError that extends the built-in Error class. Write a function that validates user input (e.g., an email address) and throws a ValidationError if the input is invalid. Use a try-catch block to handle the error and display an appropriate message to the user.
+Hint: Define a custom error class and use it within a validation function.</t>
+  </si>
+  <si>
+    <t>Asynchronous Error Handling:
+Write a function that makes an asynchronous HTTP GET request using the fetch API. Use try-catch to handle any errors that occur during the request. Ensure the function returns a meaningful error message if the request fails. Demonstrate this with a valid and an invalid URL.
+Hint: Use async/await with try-catch for asynchronous error handling.</t>
+  </si>
+  <si>
+    <t>Error Middleware in Express.js:
+Create a simple Express.js application with a few routes. Implement error-handling middleware to catch any errors that occur in the route handlers. Ensure the middleware sends a JSON response with the error message and status code. Demonstrate this by creating a route that intentionally throws an error.
+Hint: Define error-handling middleware using app.use((err, req, res, next) =&gt; { ... }).</t>
+  </si>
+  <si>
+    <t>Graceful Error Handling:
+Write a function that reads a file asynchronously using the fs.promises.readFile method. Use a try-catch block to handle any errors that occur during file reading. If an error occurs (e.g., file not found), log the error and return a default value. Demonstrate this function with an existing and a non-existing file.
+Hint: Use fs.promises.readFile inside an async function with try-catch for error handling.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2433,6 +2635,11 @@
       <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2564,7 +2771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2657,167 +2864,17 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2933,6 +2990,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2978,7 +3038,136 @@
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3218,30 +3407,6 @@
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3315,6 +3480,54 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3620,8 +3833,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D108" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:D108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D107" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:D107"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Challenge Number" dataDxfId="29"/>
     <tableColumn id="2" name="Category" dataDxfId="28"/>
@@ -3633,60 +3846,60 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C21" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="25"/>
-    <tableColumn id="2" name="Category" dataDxfId="24"/>
-    <tableColumn id="3" name="Description" dataDxfId="23"/>
+    <tableColumn id="1" name="Challenge Number" dataDxfId="23"/>
+    <tableColumn id="2" name="Category" dataDxfId="22"/>
+    <tableColumn id="3" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C21" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="20"/>
-    <tableColumn id="2" name="Category" dataDxfId="19"/>
-    <tableColumn id="3" name="Description" dataDxfId="18"/>
+    <tableColumn id="1" name="Challenge Number" dataDxfId="18"/>
+    <tableColumn id="2" name="Category" dataDxfId="17"/>
+    <tableColumn id="3" name="Description" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Category" dataDxfId="14"/>
-    <tableColumn id="3" name="Description" dataDxfId="13"/>
+    <tableColumn id="1" name="Challenge Number" dataDxfId="13"/>
+    <tableColumn id="2" name="Category" dataDxfId="12"/>
+    <tableColumn id="3" name="Description" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:C12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:C12" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A2:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Question Number" dataDxfId="3"/>
-    <tableColumn id="2" name="Category" dataDxfId="2"/>
-    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" name="Question Number" dataDxfId="7"/>
+    <tableColumn id="2" name="Category" dataDxfId="6"/>
+    <tableColumn id="3" name="Description" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:C12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A2:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Question Number" dataDxfId="9"/>
-    <tableColumn id="2" name="Category" dataDxfId="8"/>
-    <tableColumn id="3" name="Description" dataDxfId="7"/>
+    <tableColumn id="1" name="Question Number" dataDxfId="2"/>
+    <tableColumn id="2" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3957,7 +4170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -5051,10 +5264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5094,30 +5307,38 @@
       </c>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>502</v>
+      </c>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="17" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5" s="17" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
@@ -5125,7 +5346,7 @@
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>22</v>
       </c>
@@ -5135,31 +5356,41 @@
       <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="17" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="17" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="17" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="17" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
@@ -5167,7 +5398,7 @@
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>23</v>
       </c>
@@ -5177,31 +5408,41 @@
       <c r="C14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="17" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="207" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="17" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="207" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="17" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="207" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
@@ -5209,7 +5450,7 @@
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>24</v>
       </c>
@@ -5219,31 +5460,41 @@
       <c r="C20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="17" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="17" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
@@ -5251,7 +5502,7 @@
       <c r="C25" s="16"/>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -5261,33 +5512,49 @@
       <c r="C26" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="17" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="17" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="D28" s="17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="35" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="35" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>26</v>
       </c>
@@ -5297,73 +5564,93 @@
       <c r="C32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="17" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="17" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="17"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-    </row>
-    <row r="39" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
+    <row r="38" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
         <v>27</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="17"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="138" x14ac:dyDescent="0.3">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
-      <c r="D40" s="17"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D40" s="17" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="17" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="138" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
@@ -5371,22 +5658,22 @@
       <c r="C43" s="16"/>
       <c r="D43" s="17"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
+    <row r="44" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>28</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="D44" s="17"/>
     </row>
-    <row r="45" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
-        <v>28</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>55</v>
-      </c>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="17"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -5413,22 +5700,22 @@
       <c r="C49" s="16"/>
       <c r="D49" s="17"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
+    <row r="50" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>29</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="D50" s="17"/>
     </row>
-    <row r="51" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
-        <v>29</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>57</v>
-      </c>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
       <c r="D51" s="17"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -5455,22 +5742,22 @@
       <c r="C55" s="16"/>
       <c r="D55" s="17"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
+    <row r="56" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="7">
+        <v>30</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D56" s="17"/>
     </row>
-    <row r="57" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="7">
-        <v>30</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>58</v>
-      </c>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="17"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -5497,22 +5784,22 @@
       <c r="C61" s="16"/>
       <c r="D61" s="17"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
+    <row r="62" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="7">
+        <v>31</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D62" s="17"/>
     </row>
-    <row r="63" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A63" s="7">
-        <v>31</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>60</v>
-      </c>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -5539,22 +5826,22 @@
       <c r="C67" s="16"/>
       <c r="D67" s="17"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="16"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
+    <row r="68" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A68" s="7">
+        <v>32</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="D68" s="17"/>
     </row>
-    <row r="69" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A69" s="7">
-        <v>32</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>61</v>
-      </c>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="17"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -5587,22 +5874,22 @@
       <c r="C74" s="16"/>
       <c r="D74" s="17"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
+    <row r="75" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A75" s="7">
+        <v>33</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D75" s="17"/>
     </row>
-    <row r="76" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A76" s="7">
-        <v>33</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>63</v>
-      </c>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="17"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -5635,22 +5922,22 @@
       <c r="C81" s="16"/>
       <c r="D81" s="17"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="16"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
+    <row r="82" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A82" s="7">
+        <v>34</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="D82" s="17"/>
     </row>
-    <row r="83" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A83" s="7">
-        <v>34</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>65</v>
-      </c>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="16"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
       <c r="D83" s="17"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -5677,22 +5964,22 @@
       <c r="C87" s="16"/>
       <c r="D87" s="17"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="16"/>
-      <c r="B88" s="16"/>
-      <c r="C88" s="16"/>
+    <row r="88" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A88" s="7">
+        <v>35</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="D88" s="17"/>
     </row>
-    <row r="89" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A89" s="7">
-        <v>35</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>67</v>
-      </c>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
       <c r="D89" s="17"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -5719,22 +6006,22 @@
       <c r="C93" s="16"/>
       <c r="D93" s="17"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="16"/>
-      <c r="B94" s="16"/>
-      <c r="C94" s="16"/>
+    <row r="94" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A94" s="7">
+        <v>36</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="D94" s="17"/>
     </row>
-    <row r="95" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A95" s="7">
-        <v>36</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>69</v>
-      </c>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="16"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
       <c r="D95" s="17"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -5767,22 +6054,22 @@
       <c r="C100" s="16"/>
       <c r="D100" s="17"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="16"/>
-      <c r="B101" s="16"/>
-      <c r="C101" s="16"/>
+    <row r="101" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A101" s="7">
+        <v>37</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="D101" s="17"/>
     </row>
-    <row r="102" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A102" s="7">
-        <v>37</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>71</v>
-      </c>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="16"/>
+      <c r="B102" s="16"/>
+      <c r="C102" s="16"/>
       <c r="D102" s="17"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -5797,52 +6084,47 @@
       <c r="C104" s="16"/>
       <c r="D104" s="17"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="16"/>
-      <c r="B105" s="16"/>
-      <c r="C105" s="16"/>
+    <row r="105" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A105" s="7">
+        <v>38</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="D105" s="17"/>
     </row>
-    <row r="106" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A106" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D106" s="17"/>
     </row>
-    <row r="107" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D107" s="17"/>
-    </row>
-    <row r="108" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A108" s="7">
-        <v>40</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D108" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7555,7 +7837,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="221.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>84</v>
       </c>
@@ -7566,7 +7848,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>85</v>
       </c>
@@ -7577,7 +7859,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="249" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>86</v>
       </c>
@@ -7588,7 +7870,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="249" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>87</v>
       </c>
@@ -7599,7 +7881,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="235.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26">
         <v>88</v>
       </c>
@@ -7750,7 +8032,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>98</v>
       </c>
@@ -7761,7 +8043,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>99</v>
       </c>
@@ -7772,7 +8054,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
add higher order function query
</commit_message>
<xml_diff>
--- a/full-stack-challenge.xlsx
+++ b/full-stack-challenge.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Foundations of JavaScript" sheetId="1" r:id="rId1"/>
@@ -2861,14 +2861,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5266,7 +5266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="B44" sqref="B44:C75"/>
     </sheetView>
   </sheetViews>
@@ -5533,26 +5533,26 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="35" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="34" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="35" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="35"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
@@ -6641,7 +6641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
@@ -7938,11 +7938,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">

</xml_diff>

<commit_message>
add event listener Higher Order function
</commit_message>
<xml_diff>
--- a/full-stack-challenge.xlsx
+++ b/full-stack-challenge.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foundations of JavaScript" sheetId="1" r:id="rId1"/>
@@ -2385,14 +2385,6 @@
 Test the higher-order function by passing different callback functions to perform various arithmetic operations.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Event Listener Higher-Order Function
-Question: Implement a higher-order function in Kotlin that allows for easy handling of button click events across multiple views. The function should accept a lambda expression that defines what happens when a button is clicked. Demonstrate how this higher-order function simplifies adding click listeners to buttons in an Android application.</t>
-  </si>
-  <si>
-    <t>Set Operations with Higher-Order Functions
-Question: Define higher-order functions in Scheme that operate on sets represented as lists. Implement takewhile and dropwhile functions that manipulate lists based on a predicate. Provide examples demonstrating how these functions can be used to filter elements from a list according to a condition.</t>
-  </si>
-  <si>
     <t>Ordered Lists and Comparison
 Question: Develop a higher-order function in Scheme called ordered-by, which takes a comparison function as input and returns a predicate function. This predicate checks whether a given list is totally ordered according to the comparison function. Include examples showing how ordered-by can be used with different comparison functions to validate the ordering of lists.</t>
   </si>
@@ -2585,6 +2577,27 @@
     <t>Graceful Error Handling:
 Write a function that reads a file asynchronously using the fs.promises.readFile method. Use a try-catch block to handle any errors that occur during file reading. If an error occurs (e.g., file not found), log the error and return a default value. Demonstrate this function with an existing and a non-existing file.
 Hint: Use fs.promises.readFile inside an async function with try-catch for error handling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Question: Create a JavaScript function, handleButtonClick, that simplifies adding
+                                    click event listeners to buttons on a webpage. This function should accept two
+                                    parameters: a button element and a callback function. When invoked,
+                                    handleButtonClick should set up an event listener on the provided button element,
+                                    executing the callback function when the button is clicked.
+                                    Provide an example demonstrating how this function can be used to handle click
+                                    events for multiple buttons on a webpage, each triggering a different action. For
+                                    example:
+                                    Clicking "Button 1" should change the background color of the webpage.
+                                    Clicking "Button 2" should display an alert message with a custom text.
+                                    Clicking "Button 3" should toggle the visibility of a specific element on the
+                                    webpage.</t>
+  </si>
+  <si>
+    <t>Define higher-order functions in JavaScript that operate on arrays. Implement takeWhile and dropWhile functions that manipulate arrays based on a predicate. Provide examples demonstrating how these functions can be used to filter elements from an array according to a condition.
+Additionally, perform the following tasks:
+Check if it's raining OR sunny and store the result in a variable isRainingOrSunny.
+Negate the value of isRainingOrSunny and store the result in a variable notRaining.
+Display the values of isRainingOrSunny, notRaining, and isRainingAndSunny.</t>
   </si>
 </sst>
 </file>
@@ -5266,8 +5279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:C75"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5307,21 +5320,21 @@
       </c>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>502</v>
+        <v>534</v>
       </c>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="207" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>503</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
@@ -5329,7 +5342,7 @@
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
@@ -5337,7 +5350,7 @@
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5357,7 +5370,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="234.6" x14ac:dyDescent="0.3">
@@ -5365,7 +5378,7 @@
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="220.8" x14ac:dyDescent="0.3">
@@ -5373,7 +5386,7 @@
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="234.6" x14ac:dyDescent="0.3">
@@ -5381,7 +5394,7 @@
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="248.4" x14ac:dyDescent="0.3">
@@ -5389,7 +5402,7 @@
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5409,7 +5422,7 @@
         <v>47</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="220.8" x14ac:dyDescent="0.3">
@@ -5417,7 +5430,7 @@
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="207" x14ac:dyDescent="0.3">
@@ -5425,7 +5438,7 @@
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="207" x14ac:dyDescent="0.3">
@@ -5433,7 +5446,7 @@
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="207" x14ac:dyDescent="0.3">
@@ -5441,7 +5454,7 @@
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -5461,7 +5474,7 @@
         <v>49</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -5469,7 +5482,7 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
@@ -5477,7 +5490,7 @@
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="17" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="179.4" x14ac:dyDescent="0.3">
@@ -5485,7 +5498,7 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
@@ -5493,7 +5506,7 @@
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="17" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -5513,7 +5526,7 @@
         <v>51</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5521,7 +5534,7 @@
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="17" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -5529,7 +5542,7 @@
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -5537,7 +5550,7 @@
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
       <c r="D29" s="34" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
@@ -5545,7 +5558,7 @@
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
       <c r="D30" s="34" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -5565,7 +5578,7 @@
         <v>53</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
@@ -5573,7 +5586,7 @@
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
       <c r="D33" s="17" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -5581,7 +5594,7 @@
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
       <c r="D34" s="17" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -5589,7 +5602,7 @@
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
       <c r="D35" s="17" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5597,7 +5610,7 @@
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
       <c r="D36" s="17" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -5617,7 +5630,7 @@
         <v>54</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5625,7 +5638,7 @@
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
       <c r="D39" s="17" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5633,7 +5646,7 @@
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
       <c r="D40" s="17" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5641,7 +5654,7 @@
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="D41" s="17" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5649,7 +5662,7 @@
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
       <c r="D42" s="17" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -6641,8 +6654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add more questions to the bank
</commit_message>
<xml_diff>
--- a/full-stack-challenge.xlsx
+++ b/full-stack-challenge.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="650">
   <si>
     <t>Challenge Number</t>
   </si>
@@ -2925,12 +2925,234 @@
     <t>Utilizing Classic Higher-Order Functions
 Question: Without using recursion or case analysis in your definitions, create functions in JavaScript that utilize map, curry, reduce (equivalent to foldl), and reduceRight (equivalent to foldr). These functions should operate on non-empty arrays to find the maximum, sum, and product of integer elements within the array. Ensure your implementations correctly handle non-empty arrays and produce scalar results.</t>
   </si>
+  <si>
+    <t>Challenge</t>
+  </si>
+  <si>
+    <t>Simple Component Creation:
+Create a functional React component that displays a "Hello, World!" message. Convert this component into a class component and render both components in the main App component.
+Hint: Use function HelloWorld() { ... } for the functional component and class HelloWorld extends React.Component { ... } for the class component.</t>
+  </si>
+  <si>
+    <t>State Management in a Component:
+Build a simple counter application using React. Create a component that displays a counter value and two buttons to increment and decrement the counter. Use the useState hook to manage the counter state.
+Hint: Use const [count, setCount] = useState(0); to manage state in a functional component.</t>
+  </si>
+  <si>
+    <t>Event Handling:
+Create a React component with an input field and a button. Implement an event handler that updates the component's state with the current value of the input field when the button is clicked. Display the updated value below the input field.
+Hint: Use onChange event for the input field and onClick event for the button.</t>
+  </si>
+  <si>
+    <t>Lifecycle Methods:
+Implement a class component that uses lifecycle methods to log messages to the console when the component mounts and unmounts. Display a button to toggle the visibility of this component to trigger mounting and unmounting.
+Hint: Use componentDidMount and componentWillUnmount lifecycle methods in the class component.</t>
+  </si>
+  <si>
+    <t>Component Communication (Props):
+Create a parent component that passes data to a child component via props. The child component should display the data received from the parent. Implement a button in the parent component that changes the data being passed to the child component.
+Hint: Use props to pass data: &lt;ChildComponent data={this.state.data} /&gt; and access it in the child component with props.data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. State Management: Create components that read and update state from the Vuex store. Use mapState and mapMutations helpers to access state and commit mutations. Use computed properties for state and methods for mutations. &lt;br&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3. Actions and Getters: Implement actions and getters in Vuex. Create asynchronous actions to fetch data from an API and getters to compute derived state. Use mapActions and mapGetters helpers in components. &lt;br&gt; </t>
+  </si>
+  <si>
+    <t>4. Modules: Organize Vuex store into modules. Split store into separate modules for better structure and maintenance. Register modules in the main store configuration. Use namespaced option in modules. &lt;br&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Store Configuration:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Set up a Vuex store in a Vue application. Define state, mutations, actions, and getters for a simple counter. Connect the store to the Vue application. Use </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vue.use(Vuex)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>new Vuex.Store()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5. Plugin Integration: Integrate Vuex with plugins. Use Vuex plugins for additional functionality like persisting state to local storage. Create a simple plugin to log every mutation. Use store.subscribe within a plugin function.</t>
+  </si>
+  <si>
+    <t>1. Basic Routing: Set up basic routing in a Vue application. Create multiple components and configure routes to navigate between them using Vue Router. Use vue-router library and define routes in router.js. &lt;br&gt; 2. Dynamic Routing: Implement dynamic routing with parameters. Create a route that accepts an ID parameter and display corresponding details in a component. Use this.$route.params to access route parameters. &lt;br&gt; 3. Navigation Guards: Implement navigation guards. Create a guard that checks user authentication before allowing access to a route. Use beforeEnter in route configuration or global guards. &lt;br&gt; 4. Lazy Loading Routes: Implement lazy loading for routes. Configure routes to load components asynchronously to improve performance. Use () =&gt; import('path/to/component') in route definition. &lt;br&gt; 5. Nested Routes: Implement nested routes. Create a main route with nested routes for sub-components. Define nested routes within the children array in route configuration. Use router-view for nested route rendering.</t>
+  </si>
+  <si>
+    <t>1. Component Creation: Create a simple Vue component. Implement a HelloWorld component that displays a message and use it in the main App component. Use Vue.component or the component option in a Vue instance. &lt;br&gt; 2. Data Binding: Implement two-way data binding. Create a form with input fields bound to component data. Update the data as the user types. Use v-model directive for two-way binding. &lt;br&gt; 3. Event Handling: Handle user events in a Vue component. Create a button that, when clicked, updates a message displayed in the component. Use v-on directive or @click shorthand. &lt;br&gt; 4. Computed Properties: Create a computed property. Implement a computed property that returns the reversed version of a string input by the user. Use computed option in the Vue instance. &lt;br&gt; 5. Conditional Rendering: Implement conditional rendering in a Vue component. Create a component that displays different messages based on a boolean data property. Use v-if and v-else directives.</t>
+  </si>
+  <si>
+    <t>1. Creating and Providing Context: Set up a context for user authentication. Create a UserContext and a provider component that supplies user data to the application. Use React.createContext and Context.Provider. &lt;br&gt; 2. Consuming Context: Consume context data in a component. Create a component that uses the useContext hook to consume user data from UserContext. Use const user = useContext(UserContext);. &lt;br&gt; 3. Updating Context: Implement a function to update context data. Create a function within the context provider to update the user data and provide this function to consumers. Use state within the context provider and pass the state updater function. &lt;br&gt; 4. Context with Multiple Providers: Use multiple contexts in an application. Create two contexts (e.g., ThemeContext and LanguageContext) and provide them to the application. Consume both contexts in a component. Nest Context.Provider components. &lt;br&gt; 5. Context and Performance: Optimize context usage to prevent unnecessary re-renders. Memoize context values and use the useMemo hook to improve performance. Use React.memo and useMemo to optimize context updates.</t>
+  </si>
+  <si>
+    <t>1. Store Configuration: Set up a Redux store for a counter application. Create actions and reducers for incrementing and decrementing the counter. Connect the store to the React application. Use createStore and Provider from react-redux. &lt;br&gt; 2. Connecting Components: Connect a React component to the Redux store. Use useSelector to read the counter value and useDispatch to dispatch increment and decrement actions. Use const count = useSelector(state =&gt; state.count);. &lt;br&gt; 3. Async Actions with Thunk: Fetch data from an API using Redux Thunk. Create an async action to fetch data and store it in the Redux store. Display the data in a component. Use redux-thunk middleware and dispatch async actions. &lt;br&gt; 4. Redux Middleware: Create a custom middleware for logging actions. Implement a middleware that logs every action dispatched to the console. Use applyMiddleware from redux. &lt;br&gt; 5. Redux DevTools: Enable Redux DevTools in the application. Configure the Redux store to use Redux DevTools for better state management debugging. Use window.__REDUX_DEVTOOLS_EXTENSION__ in createStore.</t>
+  </si>
+  <si>
+    <t>1. Basic Routing: Implement basic routing in a React application with React Router. Create three components (Home, About, Contact) and set up routes for these components. Use BrowserRouter, Route, and Link from react-router-dom. &lt;br&gt; 2. Nested Routing: Implement nested routing in a React application. Create a component with nested routes and render different sub-components based on the URL. Use Route and useRouteMatch for nested routes. &lt;br&gt; 3. Programmatic Navigation: Implement navigation through code. Create a button that navigates to a different route when clicked using useHistory hook. Use const history = useHistory(); history.push('/route');. &lt;br&gt; 4. Route Guards: Implement a private route component. Create a private route component that redirects unauthenticated users to the login page. Use Redirect and conditional rendering in the Route component. &lt;br&gt; 5. URL Parameters: Implement a route that accepts URL parameters. Create a component that displays user details based on the user ID passed in the URL. Use useParams hook to access URL parameters.</t>
+  </si>
+  <si>
+    <t>1. State Management with useState: Create a simple todo application using the useState hook. Implement a form to add new todo items and display them in a list. Allow users to mark items as completed. Use const [todos, setTodos] = useState([]);. &lt;br&gt; 2. Side Effects with useEffect: Fetch data from an API when the component mounts using the useEffect hook. Display the fetched data in a list. Show a loading message while data is being fetched. Use useEffect(() =&gt; { fetch('url').then(...); }, []);. &lt;br&gt; 3. Context Management with useContext: Create a theme switcher using the useContext hook. Implement a context for theme management and a component to toggle between light and dark themes. Use const ThemeContext = React.createContext();. &lt;br&gt; 4. Complex State with useReducer: Implement a counter using the useReducer hook. Create a reducer function to handle increment and decrement actions and use useReducer to manage the counter state. Use const [state, dispatch] = useReducer(reducer, initialState);. &lt;br&gt; 5. Custom Hooks: Create a custom hook for form input handling. Implement a custom hook useForm that manages form state and handles input changes. Use this hook in a form component. Use function useForm(initialValues) { ... }.</t>
+  </si>
+  <si>
+    <t>1. Basic Setup: Create a new Nuxt.js project. Set up the project structure and configure basic settings for SSR. Use npx create-nuxt-app. &lt;br&gt; 2. Pages and Navigation: Create multiple pages and configure routing. Implement navigation between pages using nuxt-link. &lt;br&gt; 3. Data Fetching: Fetch data asynchronously before rendering. Use asyncData method in a page component to fetch data from an API. &lt;br&gt; 4. SEO Optimization: Implement SEO improvements. Use head property to set meta tags and titles for different pages. &lt;br&gt; 5. Deployment: Deploy the Nuxt.js application. Use a platform like Vercel or Netlify for deployment and ensure SSR is properly configured.</t>
+  </si>
+  <si>
+    <t>1. Component Creation: Create a new Angular component. Use Angular CLI to generate components and add them to the application. Use ng generate component. &lt;br&gt; 2. Data Binding: Implement data binding in a component. Use [(ngModel)] for two-way data binding and {{}} for interpolation. &lt;br&gt; 3. Event Handling: Handle user events in Angular components. Use event binding to listen for events like clicks and update component data. Use (click)="method()". &lt;br&gt; 4. Property Binding: Bind properties to component variables. Use [property]="variable" syntax for binding component properties. &lt;br&gt; 5. Component Communication: Implement parent-child communication using Input and Output decorators. Pass data between parent and child components using @Input and @Output.</t>
+  </si>
+  <si>
+    <t>1. Service Creation: Create an Angular service. Use Angular CLI to generate a service and inject it into a component. Use ng generate service. &lt;br&gt; 2. Dependency Injection: Inject the service into multiple components. Use constructor injection to provide the service instance to components. &lt;br&gt; 3. HTTP Requests: Use Angular HttpClient in a service to fetch data from an API. Import HttpClientModule and use HttpClient to make GET and POST requests. &lt;br&gt; 4. Shared Logic: Move shared logic to the service. Refactor business logic from components into a service and use the service methods in components. &lt;br&gt; 5. Observable and RxJS: Implement data sharing using RxJS observables. Use BehaviorSubject to manage and share state across components.</t>
+  </si>
+  <si>
+    <t>1. Router Setup: Set up Angular Router in an application. Import RouterModule and define routes in the AppRoutingModule. &lt;br&gt; 2. Basic Navigation: Create routes for different components. Use routerLink directive for navigation. Use RouterModule.forRoot() to configure routes. &lt;br&gt; 3. Route Parameters: Implement dynamic routing with route parameters. Create a route with parameters and access them in the component using ActivatedRoute. &lt;br&gt; 4. Lazy Loading: Implement lazy loading for modules. Configure the router to load feature modules lazily using loadChildren. &lt;br&gt; 5. Route Guards: Implement route guards for authentication. Create an AuthGuard and protect routes based on user authentication status.</t>
+  </si>
+  <si>
+    <t>1. Template-Driven Forms: Create a template-driven form. Use ngModel for two-way data binding and handle form submission. Use FormsModule for template-driven forms. &lt;br&gt; 2. Reactive Forms: Create a reactive form. Use FormBuilder to create form controls and group them into a form group. Use ReactiveFormsModule for reactive forms. &lt;br&gt; 3. Form Validation: Implement form validation. Add validation rules to form controls and display validation messages in the template. Use Validators class for validation. &lt;br&gt; 4. Custom Validators: Create custom validators. Implement a custom validator function and apply it to form controls. &lt;br&gt; 5. Form Submission: Handle form submission. Write a method to process form data and submit it to a backend service. Use ngSubmit directive for handling form submission.</t>
+  </si>
+  <si>
+    <t>1. Directive Creation: Create a new custom directive. Use Angular CLI to generate a directive and implement basic functionality. Use ng generate directive. &lt;br&gt; 2. Attribute Directive: Implement an attribute directive. Create a directive that changes the background color of an element. Use Renderer2 and ElementRef for DOM manipulation. &lt;br&gt; 3. Structural Directive: Create a structural directive. Implement a directive that conditionally adds or removes an element from the DOM. Use TemplateRef and ViewContainerRef. &lt;br&gt; 4. HostListener and HostBinding: Use HostListener and HostBinding decorators. Handle events and bind properties in a directive. &lt;br&gt; 5. Directive Input: Pass data to directives using @Input. Create a directive that accepts input properties and uses them to modify element behavior.</t>
+  </si>
+  <si>
+    <t>1. Basic Setup: Set up a new Next.js project. Create pages and configure routing using the file-based routing system. Use npx create-next-app. &lt;br&gt; 2. Data Fetching: Implement data fetching methods. Use getServerSideProps and getStaticProps to fetch data at build time or request time. &lt;br&gt; 3. API Routes: Create API routes in Next.js. Implement serverless functions within the api directory to handle backend logic. &lt;br&gt; 4. Dynamic Routes: Implement dynamic routing. Create dynamic pages using file and folder naming conventions with square brackets. &lt;br&gt; 5. Deployment: Deploy the Next.js application. Use Vercel or another platform for deployment and ensure proper SSR setup.</t>
+  </si>
+  <si>
+    <t>1. Basic Setup: Create a new Gatsby.js project. Set up the project structure and install necessary plugins. Use gatsby new. &lt;br&gt; 2. Pages and Navigation: Create pages and configure routing. Use Link from gatsby for navigation and gatsby-node.js for programmatic page creation. &lt;br&gt; 3. Data Sources: Fetch data from various sources using GraphQL. Configure source plugins to fetch data from Markdown files, CMS, or APIs. &lt;br&gt; 4. SEO Optimization: Implement SEO improvements. Use gatsby-plugin-react-helmet to manage meta tags and improve SEO. &lt;br&gt; 5. Deployment: Deploy the Gatsby.js site. Use platforms like Netlify or Vercel for deployment and ensure static site optimization.</t>
+  </si>
+  <si>
+    <t>1. Component Creation: Create a new Svelte component. Implement a HelloWorld component and use it in the main App component. Use svelte for development. &lt;br&gt; 2. Reactive Declarations: Implement reactive declarations. Use $: syntax to create reactive statements that update automatically. &lt;br&gt; 3. Event Handling: Handle events in Svelte components. Create a button that updates a message when clicked. Use on:click directive. &lt;br&gt; 4. Two-Way Binding: Implement two-way data binding. Use bind: directive to bind component data to form inputs. &lt;br&gt; 5. Component Props: Pass data to components using props. Create a parent component that passes data to a child component using export let.</t>
+  </si>
+  <si>
+    <t>1. Writable Store: Create a writable store. Use writable from svelte/store to manage a counter state. Use const count = writable(0);. &lt;br&gt; 2. Readable Store: Implement a readable store. Create a store that provides read-only access to data, such as current time. Use const time = readable(new Date(), set =&gt; { ... });. &lt;br&gt; 3. Custom Store: Create a custom store. Implement a store with custom methods for updating state. Use function createCustomStore() { ... }. &lt;br&gt; 4. Store Subscription: Subscribe to store updates in components. Use $store syntax to auto-subscribe and update component state. &lt;br&gt; 5. Derived Store: Create a derived store. Combine multiple stores into a single derived store that computes derived state. Use derived from svelte/store.</t>
+  </si>
+  <si>
+    <t>1. Router Setup: Set up basic routing in a Svelte application. Use svelte-routing library and configure routes using &lt;Router&gt; and &lt;Route&gt;. &lt;br&gt; 2. Nested Routes: Implement nested routes. Create a parent route with nested child routes and render different components based on the nested route. &lt;br&gt; 3. Route Parameters: Implement dynamic routing with route parameters. Create routes that accept parameters and access them in components using params. &lt;br&gt; 4. Route Guards: Implement navigation guards. Protect routes based on authentication status and redirect unauthenticated users. &lt;br&gt; 5. Lazy Loading: Implement lazy loading for routes. Load components asynchronously to improve performance. Use import function for dynamic imports.</t>
+  </si>
+  <si>
+    <t>1. Scene Setup: Create a basic Three.js scene. Set up a scene, camera, and renderer to display a 3D object. Use THREE.Scene, THREE.PerspectiveCamera, and THREE.WebGLRenderer. &lt;br&gt; 2. Basic Geometry: Add basic geometry to the scene. Create and add shapes like cubes, spheres, and planes. Use THREE.BoxGeometry, THREE.SphereGeometry. &lt;br&gt; 3. Materials and Textures: Apply materials and textures to objects. Use different material types and load textures from images. Use THREE.MeshBasicMaterial, THREE.TextureLoader. &lt;br&gt; 4. Animation Loop: Implement an animation loop. Create a loop to render the scene continuously and update object properties for animation. Use requestAnimationFrame and update within the loop. &lt;br&gt; 5. Lighting: Add lighting to the scene. Implement different light types such as ambient, directional, and point lights. Use THREE.AmbientLight, THREE.DirectionalLight.</t>
+  </si>
+  <si>
+    <t>1. Basic Setup: Create a new web worker. Write a JavaScript file for the worker and instantiate it in the main script using new Worker('worker.js'). &lt;br&gt; 2. Message Passing: Implement communication between the main thread and the web worker. Use postMessage and onmessage to send and receive messages. &lt;br&gt; 3. Data Processing: Offload a computationally intensive task to the web worker. Write logic in the worker script to process data and return results. &lt;br&gt; 4. Error Handling: Implement error handling in the worker. Use onerror to catch errors in the worker and handle them gracefully. &lt;br&gt; 5. Terminating Workers: Terminate the web worker when it's no longer needed. Use worker.terminate() to stop the worker and free up resources.</t>
+  </si>
+  <si>
+    <t>1. Registration: Register a service worker in the main script. Use navigator.serviceWorker.register('/service-worker.js') to register the worker. &lt;br&gt; 2. Caching Strategies: Implement different caching strategies. Use Cache API to cache assets and resources during the install event. &lt;br&gt; 3. Offline Support: Enable offline support. Write logic in the service worker to serve cached content when the network is unavailable. &lt;br&gt; 4. Push Notifications: Implement push notifications. Use Push API to subscribe to push notifications and display them using the Notification API. &lt;br&gt; 5. Update Handling: Handle service worker updates. Implement logic to detect and activate new service worker versions without disrupting the user experience.</t>
+  </si>
+  <si>
+    <t>1. Manifest File: Create a web app manifest file. Define metadata like the app name, icons, and start URL in manifest.json. &lt;br&gt; 2. Service Worker Setup: Register a service worker for offline capabilities. Use the service worker to cache assets and enable offline functionality. &lt;br&gt; 3. Installability: Make the app installable. Ensure the web app meets PWA criteria and is prompted for installation by browsers. &lt;br&gt; 4. Testing: Test PWA features. Use tools like Lighthouse in Chrome DevTools to test and optimize PWA performance. &lt;br&gt; 5. Deployment: Deploy the PWA. Ensure the PWA is served over HTTPS and verify its functionality in different environments.</t>
+  </si>
+  <si>
+    <t>1. WebSocket Setup: Establish a WebSocket connection. Create a WebSocket server and client to exchange messages in real-time. Use new WebSocket('ws://server'). &lt;br&gt; 2. Message Handling: Implement message handling in WebSockets. Write server and client logic to handle incoming and outgoing messages. &lt;br&gt; 3. SSE Setup: Set up Server-Sent Events. Create an SSE endpoint on the server and subscribe to it on the client using EventSource. &lt;br&gt; 4. Real-Time Updates: Implement real-time updates using WebSockets or SSE. Use these technologies to push real-time data updates to clients. &lt;br&gt; 5. Error Handling: Handle errors and reconnections in WebSockets and SSE. Implement logic to detect disconnections and attempt reconnection.</t>
+  </si>
+  <si>
+    <t>1. Basic Setup: Set up a GraphQL server. Use a GraphQL server library like Apollo Server to define schemas and resolvers. &lt;br&gt; 2. Client Integration: Integrate GraphQL on the client side. Use Apollo Client or Relay to fetch data from the GraphQL server. &lt;br&gt; 3. Queries: Write GraphQL queries to fetch data. Define and execute queries to retrieve specific data required by the client. &lt;br&gt; 4. Mutations: Implement GraphQL mutations to modify data. Write mutation resolvers on the server and call them from the client. &lt;br&gt; 5. Subscriptions: Implement real-time updates with GraphQL subscriptions. Set up a subscription server to push real-time data to clients.</t>
+  </si>
+  <si>
+    <t>1. Basic Setup: Establish a WebRTC connection. Use RTCPeerConnection to create a peer-to-peer connection between clients. &lt;br&gt; 2. Media Streams: Capture media streams. Use getUserMedia to access the device's camera and microphone and add the streams to the peer connection. &lt;br&gt; 3. Signaling: Implement a signaling mechanism. Use a signaling server to exchange session descriptions (SDP) and ICE candidates between peers. &lt;br&gt; 4. Data Channels: Create a data channel for file sharing. Use RTCDataChannel to send and receive arbitrary data between peers. &lt;br&gt; 5. Error Handling: Handle errors and disconnections in WebRTC. Implement logic to detect and recover from connection issues and handle media stream errors.</t>
+  </si>
+  <si>
+    <t>1. Compilation: Compile C/C++ code to WebAssembly. Use Emscripten to compile source code into a WebAssembly module (.wasm file). &lt;br&gt; 2. Loading Module: Load and instantiate the WebAssembly module in JavaScript. Use WebAssembly.instantiate to load the .wasm file. &lt;br&gt; 3. Memory Management: Manage memory for WebAssembly. Allocate and deallocate memory for data exchange between JavaScript and WebAssembly. &lt;br&gt; 4. Interfacing: Interface between JavaScript and WebAssembly. Call exported WebAssembly functions from JavaScript and pass arguments. &lt;br&gt; 5. Optimization: Optimize WebAssembly performance. Use compiler optimization flags and techniques to improve the performance of the WebAssembly module.</t>
+  </si>
+  <si>
+    <t>1. Proposal Research: Research and choose an ECMAScript proposal. Select a stage-3 or higher proposal from TC39's process. &lt;br&gt; 2. Polyfill Implementation: Implement a polyfill for the proposal. Write JavaScript code to mimic the behavior of the proposed feature. &lt;br&gt; 3. Testing: Test the new feature. Write unit tests to verify the correctness and compatibility of the polyfill. &lt;br&gt; 4. Integration: Integrate the polyfill into a project. Use the polyfill in a real-world application to test its practicality and performance. &lt;br&gt; 5. Feedback: Provide feedback to the proposal authors. Share findings and suggestions based on the implementation experience with the TC39 community.</t>
+  </si>
+  <si>
+    <t>1. Garbage Collection: Learn about JavaScript garbage collection. Understand how V8 and other engines manage memory and perform garbage collection. &lt;br&gt; 2. Memory Leaks: Identify common causes of memory leaks. Analyze code patterns that lead to memory leaks, such as circular references and detached DOM nodes. &lt;br&gt; 3. Profiling: Use memory profiling tools. Utilize browser developer tools to profile memory usage and detect leaks in web applications. &lt;br&gt; 4. Optimization Techniques: Implement memory optimization techniques. Apply best practices like object pooling, efficient data structures, and lazy loading. &lt;br&gt; 5. Performance Monitoring: Monitor and analyze memory performance. Set up monitoring tools to track memory usage and optimize based on real-time data.</t>
+  </si>
+  <si>
+    <t>1. Factory Pattern: Implement the Factory pattern. Create a factory function that returns different types of objects based on input parameters. &lt;br&gt; 2. Observer Pattern: Implement the Observer pattern. Create a subject that maintains a list of observers and notifies them of state changes. &lt;br&gt; 3. Decorator Pattern: Implement the Decorator pattern. Enhance object behavior dynamically by wrapping objects with decorator functions. &lt;br&gt; 4. Proxy Pattern: Implement the Proxy pattern. Use the Proxy object to control access and modifications to another object. &lt;br&gt; 5. Practical Application: Apply design patterns in a project. Integrate these patterns into a real-world application to solve specific design problems.</t>
+  </si>
+  <si>
+    <t>1. Functors: Understand and implement functors. Create a functor class that implements the map method to apply functions to wrapped values. &lt;br&gt; 2. Monads: Learn about monads and implement them. Create a monad class that implements flatMap (or chain) for function composition. &lt;br&gt; 3. Monoids: Implement monoids. Create a monoid class that implements an associative binary operation and an identity element. &lt;br&gt; 4. Higher-Order Functions: Use higher-order functions. Write functions that take other functions as arguments or return them. &lt;br&gt; 5. Real-World Usage: Apply functional programming in real-world scenarios. Refactor existing codebases to use functional patterns for improved maintainability.</t>
+  </si>
+  <si>
+    <t>1. Concurrency Models: Understand JavaScript's concurrency model. Learn about the event loop, call stack, and task queue. &lt;br&gt; 2. Web Workers: Use web workers for parallelism. Offload tasks to web workers to run them in parallel with the main thread. &lt;br&gt; 3. Async/Await: Implement asynchronous code using async and await. Write non-blocking code that handles asynchronous operations seamlessly. &lt;br&gt; 4. Promises: Use Promises for concurrency. Chain and handle multiple asynchronous operations with Promises. &lt;br&gt; 5. Parallel Processing: Explore parallel processing libraries. Use libraries like parallel.js to execute tasks in parallel across multiple threads.</t>
+  </si>
+  <si>
+    <t>1. Service Decomposition: Decompose a monolithic application into microservices. Identify and separate functionalities into independent services. &lt;br&gt; 2. Communication: Implement communication between microservices. Use HTTP, gRPC, or message queues for inter-service communication. &lt;br&gt; 3. API Gateway: Set up an API Gateway. Use an API Gateway to manage and route requests to the appropriate microservices. &lt;br&gt; 4. Service Discovery: Implement service discovery. Use tools like Consul or Eureka for dynamic discovery and registration of services. &lt;br&gt; 5. Deployment: Deploy microservices. Use containerization tools like Docker and orchestration platforms like Kubernetes for scalable deployment.</t>
+  </si>
+  <si>
+    <t>1. Architecture Design: Design the architecture of a distributed system. Understand and plan for horizontal scaling, data partitioning, and redundancy. &lt;br&gt; 2. Distributed Databases: Implement distributed databases. Use databases like Cassandra, MongoDB, or DynamoDB for data distribution and replication. &lt;br&gt; 3. Consistency Models: Understand consistency models. Learn about eventual consistency, strong consistency, and CAP theorem. &lt;br&gt; 4. Fault Tolerance: Implement fault tolerance mechanisms. Use techniques like replication, sharding, and consensus algorithms (e.g., Raft, Paxos). &lt;br&gt; 5. Monitoring: Set up monitoring and logging. Use tools like Prometheus, Grafana, and ELK stack for monitoring and analyzing system performance.</t>
+  </si>
+  <si>
+    <t>1. Observable Creation: Create observables. Use RxJS to create observables that emit data over time. &lt;br&gt; 2. Operators: Use RxJS operators. Apply operators like map, filter, merge, and switchMap to transform and combine observables. &lt;br&gt; 3. Subscription: Implement subscription logic. Subscribe to observables to react to emitted data and handle it in the application. &lt;br&gt; 4. Error Handling: Handle errors in observables. Use RxJS error handling operators like catchError and retry to manage errors in data streams. &lt;br&gt; 5. Real-World Application: Integrate RxJS into a real-world application. Use reactive programming to manage complex asynchronous data flows.</t>
+  </si>
+  <si>
+    <t>1. Blockchain Basics: Understand blockchain technology. Learn about the fundamental concepts of blockchain, including blocks, transactions, and consensus. &lt;br&gt; 2. Ethereum Integration: Integrate Ethereum blockchain. Use Ethereum.js to interact with Ethereum blockchain, deploy smart contracts, and manage transactions. &lt;br&gt; 3. Smart Contracts: Write and deploy smart contracts. Use Solidity to write smart contracts and deploy them on the Ethereum network. &lt;br&gt; 4. DApp Development: Develop decentralized applications (DApps). Build a frontend interface that interacts with smart contracts and blockchain data. &lt;br&gt; 5. Security: Implement security best practices. Ensure the security of blockchain transactions and smart contracts by following best practices and auditing code.</t>
+  </si>
+  <si>
+    <t>1. TensorFlow.js Setup: Set up TensorFlow.js. Install and configure TensorFlow.js for running machine learning models in the browser. &lt;br&gt; 2. Model Training: Train machine learning models. Use TensorFlow.js to define, train, and evaluate models for tasks like classification and regression. &lt;br&gt; 3. Pre-trained Models: Use pre-trained models. Load and use pre-trained models from TensorFlow Hub for common tasks like image recognition and text analysis. &lt;br&gt; 4. Inference: Perform inference with models. Use trained models to make predictions on new data in real-time. &lt;br&gt; 5. Integration: Integrate AI into web applications. Build interactive web apps that utilize machine learning models for intelligent features.</t>
+  </si>
+  <si>
+    <t>1. Quantum Basics: Learn the basics of quantum computing. Understand qubits, superposition, entanglement, and quantum gates. &lt;br&gt; 2. Quantum Libraries: Explore JavaScript libraries for quantum computing, such as Quantum JavaScript (jsqubits). Understand how to simulate basic quantum circuits. &lt;br&gt; 3. Quantum Circuits: Create quantum circuits. Use JavaScript libraries to define quantum circuits and run them on quantum simulators or real quantum hardware. &lt;br&gt; 4. Algorithms: Implement quantum algorithms. Write and test quantum algorithms like Grover's search and Shor's factoring. &lt;br&gt; 5. Applications: Explore quantum applications. Research and develop potential applications of quantum computing in areas like cryptography and optimization.</t>
+  </si>
+  <si>
+    <t>1. AR Setup: Set up AR.js for augmented reality development. Configure the environment and include necessary scripts for AR functionality. &lt;br&gt; 2. Marker-Based AR: Implement marker-based AR. Use AR.js to detect and track markers, and overlay 3D content on them. &lt;br&gt; 3. Markerless AR: Explore markerless AR. Implement AR experiences that do not rely on physical markers, using device sensors and computer vision. &lt;br&gt; 4. 3D Content: Create and display 3D content in AR. Use 3D models and animations to enhance the AR experience. &lt;br&gt; 5. User Interaction: Implement user interaction in AR. Enable interactions like tapping, dragging, and resizing AR objects using JavaScript event listeners.</t>
+  </si>
+  <si>
+    <t>1. VR Setup: Set up A-Frame for VR development. Include A-Frame library and create a basic VR scene with essential components. &lt;br&gt; 2. Scene Creation: Create complex VR scenes. Use A-Frame primitives and custom components to build immersive VR environments. &lt;br&gt; 3. Interactions: Implement user interactions in VR. Use controllers and event listeners to enable user interaction with VR elements. &lt;br&gt; 4. Animations: Add animations to VR objects. Use A-Frame's animation components to create dynamic and engaging VR experiences. &lt;br&gt; 5. Performance Optimization: Optimize VR performance. Ensure smooth rendering and performance by optimizing assets and using efficient coding practices.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2979,6 +3201,24 @@
       <sz val="9.6"/>
       <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3110,7 +3350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3206,17 +3446,226 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3869,126 +4318,6 @@
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4162,86 +4491,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D122" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D122" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:D122"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="35"/>
-    <tableColumn id="2" name="Category" dataDxfId="34"/>
-    <tableColumn id="3" name="Description" dataDxfId="33"/>
-    <tableColumn id="4" name="Task" dataDxfId="32"/>
+    <tableColumn id="1" name="Challenge Number" dataDxfId="37"/>
+    <tableColumn id="2" name="Category" dataDxfId="36"/>
+    <tableColumn id="3" name="Description" dataDxfId="35"/>
+    <tableColumn id="4" name="Task" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D120" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D120" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:D120"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="29"/>
-    <tableColumn id="2" name="Category" dataDxfId="28"/>
-    <tableColumn id="3" name="Description" dataDxfId="27"/>
-    <tableColumn id="4" name="Task" dataDxfId="26"/>
+    <tableColumn id="1" name="Challenge Number" dataDxfId="31"/>
+    <tableColumn id="2" name="Category" dataDxfId="30"/>
+    <tableColumn id="3" name="Description" dataDxfId="29"/>
+    <tableColumn id="4" name="Task" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A1:C21"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="23"/>
-    <tableColumn id="2" name="Category" dataDxfId="22"/>
-    <tableColumn id="3" name="Description" dataDxfId="21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D21" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D21"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Challenge Number" dataDxfId="3"/>
+    <tableColumn id="2" name="Category" dataDxfId="2"/>
+    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" name="Task" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:C21"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="18"/>
-    <tableColumn id="2" name="Category" dataDxfId="17"/>
-    <tableColumn id="3" name="Description" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D32" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:D32"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Challenge Number" dataDxfId="25"/>
+    <tableColumn id="2" name="Category" dataDxfId="24"/>
+    <tableColumn id="3" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" name="Challenge" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C21" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Challenge Number" dataDxfId="13"/>
-    <tableColumn id="2" name="Category" dataDxfId="12"/>
-    <tableColumn id="3" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" name="Challenge Number" dataDxfId="20"/>
+    <tableColumn id="2" name="Category" dataDxfId="19"/>
+    <tableColumn id="3" name="Description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:C12" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:C12" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A2:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Question Number" dataDxfId="7"/>
-    <tableColumn id="2" name="Category" dataDxfId="6"/>
-    <tableColumn id="3" name="Description" dataDxfId="5"/>
+    <tableColumn id="1" name="Question Number" dataDxfId="14"/>
+    <tableColumn id="2" name="Category" dataDxfId="13"/>
+    <tableColumn id="3" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:C12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Question Number" dataDxfId="2"/>
-    <tableColumn id="2" name="Category" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Question Number" dataDxfId="9"/>
+    <tableColumn id="2" name="Category" dataDxfId="8"/>
+    <tableColumn id="3" name="Description" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4512,7 +4843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="B29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -5602,7 +5933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -6264,7 +6595,7 @@
       <c r="C74" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D74" s="36" t="s">
+      <c r="D74" s="35" t="s">
         <v>538</v>
       </c>
     </row>
@@ -6675,20 +7006,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -6698,8 +7030,11 @@
       <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D1" s="44" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>41</v>
       </c>
@@ -6709,8 +7044,11 @@
       <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D2" s="42" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>42</v>
       </c>
@@ -6720,8 +7058,11 @@
       <c r="C3" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D3" s="42" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>43</v>
       </c>
@@ -6731,8 +7072,11 @@
       <c r="C4" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D4" s="42" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>44</v>
       </c>
@@ -6742,8 +7086,11 @@
       <c r="C5" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D5" s="42" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>45</v>
       </c>
@@ -6753,8 +7100,11 @@
       <c r="C6" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D6" s="42" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>46</v>
       </c>
@@ -6764,8 +7114,11 @@
       <c r="C7" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D7" s="42" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>47</v>
       </c>
@@ -6775,8 +7128,11 @@
       <c r="C8" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D8" s="42" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>48</v>
       </c>
@@ -6786,8 +7142,11 @@
       <c r="C9" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D9" s="42" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>49</v>
       </c>
@@ -6797,8 +7156,11 @@
       <c r="C10" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D10" s="42" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>50</v>
       </c>
@@ -6808,8 +7170,11 @@
       <c r="C11" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D11" s="42" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>51</v>
       </c>
@@ -6819,8 +7184,11 @@
       <c r="C12" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D12" s="42" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>52</v>
       </c>
@@ -6830,8 +7198,11 @@
       <c r="C13" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D13" s="42" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>53</v>
       </c>
@@ -6841,8 +7212,11 @@
       <c r="C14" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D14" s="42" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>54</v>
       </c>
@@ -6852,8 +7226,11 @@
       <c r="C15" s="7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D15" s="42" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>55</v>
       </c>
@@ -6863,8 +7240,11 @@
       <c r="C16" s="7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D16" s="42" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>56</v>
       </c>
@@ -6874,8 +7254,11 @@
       <c r="C17" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D17" s="42" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>57</v>
       </c>
@@ -6885,8 +7268,11 @@
       <c r="C18" s="7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D18" s="42" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>58</v>
       </c>
@@ -6896,8 +7282,11 @@
       <c r="C19" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="42" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>59</v>
       </c>
@@ -6907,8 +7296,11 @@
       <c r="C20" s="7" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="42" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>60</v>
       </c>
@@ -6917,6 +7309,9 @@
       </c>
       <c r="C21" s="7" t="s">
         <v>116</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -6929,10 +7324,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C21"/>
+    <sheetView topLeftCell="D11" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6940,9 +7335,10 @@
     <col min="1" max="1" width="18.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
     <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="64.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -6952,8 +7348,11 @@
       <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D1" s="38" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>61</v>
       </c>
@@ -6963,220 +7362,365 @@
       <c r="C2" s="25" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
+      <c r="D2" s="39" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+    </row>
+    <row r="8" spans="1:4" ht="234.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
         <v>62</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B8" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C8" s="25" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="25">
+      <c r="D8" s="40" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
         <v>63</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B9" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C9" s="25" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="D9" s="40" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="207" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
         <v>64</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B10" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C10" s="25" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
+      <c r="D10" s="40" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
         <v>65</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B11" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C11" s="25" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
+      <c r="D11" s="40" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
         <v>66</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B12" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C12" s="25" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="25">
+      <c r="D12" s="40" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
         <v>67</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B13" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C13" s="25" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
+      <c r="D13" s="40" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
         <v>68</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B14" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C14" s="25" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
+      <c r="D14" s="41" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="40" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="40" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="40" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
+    </row>
+    <row r="20" spans="1:4" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="25">
         <v>69</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B20" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C20" s="25" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+      <c r="D20" s="45" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="25">
         <v>70</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B21" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C21" s="25" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
+      <c r="D21" s="45" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="25">
         <v>71</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B22" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C22" s="25" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="D22" s="45" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="25">
         <v>72</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B23" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C23" s="25" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
+      <c r="D23" s="45" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="25">
         <v>73</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B24" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="D24" s="45" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="25">
         <v>74</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B25" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
+      <c r="D25" s="45" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25">
         <v>75</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B26" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C26" s="25" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+      <c r="D26" s="45" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="25">
         <v>76</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B27" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C27" s="25" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
+      <c r="D27" s="45" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="25">
         <v>77</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B28" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C28" s="25" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="D28" s="45" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="25">
         <v>78</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B29" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C29" s="25" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
+      <c r="D29" s="45" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="25">
         <v>79</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B30" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C30" s="25" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
+      <c r="D30" s="45" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25">
         <v>80</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B31" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C31" s="25" t="s">
         <v>156</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="43" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7444,6 +7988,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="19" max="19" width="16.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
@@ -8188,7 +8735,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8482,11 +9029,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">

</xml_diff>